<commit_message>
Adding The condition of the Threshold
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5dc51053675dbbaa/Documents/UiPath/Academy-Ref-UiDemo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E410E0A2-CC01-42FC-AF7D-B9D0AFAD38C3}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1B8A09A-EFE0-4B9A-9072-089C4DBDEA51}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,10 +174,10 @@
     <t>UiDemo_Credential</t>
   </si>
   <si>
-    <t>ManualTransactionTreshold</t>
-  </si>
-  <si>
     <t>FALSE</t>
+  </si>
+  <si>
+    <t>ManualTransactionThreshold</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -658,7 +658,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>10000</v>
@@ -1841,7 +1841,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>41</v>

</xml_diff>